<commit_message>
added comments; wrote doc
</commit_message>
<xml_diff>
--- a/Doc/comparison.xlsx
+++ b/Doc/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82098423df8d287f/data/Uni/CSDC/01_3Semester/AI/Bublin/8Puzzle/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{2AB5A1D3-7F8A-4204-BB5F-D2AAF22A71EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0ED79F9-C6FF-4816-A996-1AE5E43ED359}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{2AB5A1D3-7F8A-4204-BB5F-D2AAF22A71EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DA5C1D5-AF62-4730-8EC5-B7CFEE2ED48C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{048E2764-DD61-425F-8AF1-B98D862D6EF2}"/>
   </bookViews>
@@ -18,6 +18,17 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$B$1:$B$236</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Tabelle1!$D$1:$D$236</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Tabelle1!$E$1:$E$236</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Tabelle1!$P$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Tabelle1!$B$1:$B$236</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Tabelle1!$C$1:$C$236</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Tabelle1!$D$1:$D$236</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Tabelle1!$E$1:$E$236</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Tabelle1!$P$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -112,7 +123,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Iterations Hemming</c:v>
+            <c:v>Iterations Hamming</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2564,7 +2575,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Time Hemming</c:v>
+            <c:v>Time Hamming</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -5025,6 +5036,117 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{7B437D17-BAEF-4222-B681-165F02271286}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Iterations Hamming</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000002-3165-4DC3-9814-A3D64A15AB54}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Iterations Manhatten</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000000-C298-4087-9459-6CDD15A012DC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Time Hamming</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-C298-4087-9459-6CDD15A012DC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Time Manhatten</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5066,6 +5188,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6137,6 +6339,1036 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6213,6 +7445,162 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>372340</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100444</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>320386</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>86589</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Diagramm 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44524E83-E00A-9D29-2610-0316996A5704}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11040340" y="100444"/>
+              <a:ext cx="6044046" cy="3804805"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-AT" sz="1100"/>
+                <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
+Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>320386</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>268432</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>46760</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Diagramm 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21D49E72-88B3-46E7-A1F2-927E03F674FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10988386" y="4061115"/>
+              <a:ext cx="6044046" cy="3804805"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-AT" sz="1100"/>
+                <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
+Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10543,8 +11931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431CA064-68E5-4533-9665-D159C80448BF}">
   <dimension ref="A1:E236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>